<commit_message>
docs: add comparison to previous data
</commit_message>
<xml_diff>
--- a/results/99_manuscript_figures/SupplementaryTable2_ldsc_global.xlsx
+++ b/results/99_manuscript_figures/SupplementaryTable2_ldsc_global.xlsx
@@ -7,13 +7,17 @@
   </bookViews>
   <sheets>
     <sheet name="column_descriptions" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="results" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="trait_h2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="global_rg" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+  <si>
+    <t xml:space="preserve">sheet</t>
+  </si>
   <si>
     <t xml:space="preserve">column_name</t>
   </si>
@@ -21,6 +25,60 @@
     <t xml:space="preserve">description</t>
   </si>
   <si>
+    <t xml:space="preserve">trait_h2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phenotype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total_observed_scale_h2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimated SNP heritability (h2, observed scale)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total_observed_scale_h2_se</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard error of h2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lambda_gc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genomic inflation factor (lambda GC); equivalent of median(chi^2)/0.4549, where denominator indicates expected median of the chi-squared distribution with 1 degree of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean_chi_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean chi-square statistic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intercept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LD score regression intercept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intercept_se</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard error for LD score regression intercept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heritability Z-score (equivalent of h2/se)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">global_rg</t>
+  </si>
+  <si>
     <t xml:space="preserve">p1</t>
   </si>
   <si>
@@ -45,9 +103,6 @@
     <t xml:space="preserve">The bootstrap standard error of the genetic correlation estimate</t>
   </si>
   <si>
-    <t xml:space="preserve">z</t>
-  </si>
-  <si>
     <t xml:space="preserve">p</t>
   </si>
   <si>
@@ -57,7 +112,7 @@
     <t xml:space="preserve">h2_obs</t>
   </si>
   <si>
-    <t xml:space="preserve">Estimated snp-heritability of the second phenotype </t>
+    <t xml:space="preserve">Estimated SNP heritability (h2, observed scale) of the second phenotype </t>
   </si>
   <si>
     <t xml:space="preserve">h2_obs_se</t>
@@ -93,6 +148,9 @@
     <t xml:space="preserve">AD2019</t>
   </si>
   <si>
+    <t xml:space="preserve">AD2019.Kunkle</t>
+  </si>
+  <si>
     <t xml:space="preserve">BIP2021</t>
   </si>
   <si>
@@ -100,6 +158,9 @@
   </si>
   <si>
     <t xml:space="preserve">MDD2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD2019.ex23andMe.exUKBB</t>
   </si>
   <si>
     <t xml:space="preserve">PD2019.meta5.ex23andMe</t>
@@ -453,101 +514,228 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -568,48 +756,298 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.0021</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.0864</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.1254</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1.0027</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0108</v>
+      </c>
+      <c r="H2" t="n">
+        <v>7.14285714285714</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.0713</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0114</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.0926</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.118</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1.0302</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0084</v>
+      </c>
+      <c r="H3" t="n">
+        <v>6.25438596491228</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.0708</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0027</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.453</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.5926</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1.0247</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0089</v>
+      </c>
+      <c r="H4" t="n">
+        <v>26.2222222222222</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.1711</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0755</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.0225</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.0245</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1.002</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.0071</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2.26622516556291</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.0598</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0023</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.453</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1.5893</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.0017</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.0098</v>
+      </c>
+      <c r="H6" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.3062</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0275</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.0679</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.0928</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.977</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0057</v>
+      </c>
+      <c r="H7" t="n">
+        <v>11.1345454545455</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.0186</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0017</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.0895</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.136</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.9838</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0065</v>
+      </c>
+      <c r="H8" t="n">
+        <v>10.9411764705882</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.4101</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0138</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.6831</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.932</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1.0699</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0113</v>
+      </c>
+      <c r="H9" t="n">
+        <v>29.7173913043478</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -644,10 +1082,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C3" t="n">
         <v>0.1266</v>
@@ -682,10 +1120,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C4" t="n">
         <v>0.3769</v>
@@ -720,10 +1158,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C5" t="n">
         <v>0.1696</v>
@@ -758,10 +1196,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C6" t="n">
         <v>0.1973</v>
@@ -796,10 +1234,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C7" t="n">
         <v>0.1087</v>
@@ -834,10 +1272,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C8" t="n">
         <v>0.1266</v>
@@ -872,10 +1310,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C9" t="n">
         <v>1</v>
@@ -910,10 +1348,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C10" t="n">
         <v>-0.1158</v>
@@ -948,10 +1386,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C11" t="n">
         <v>0.4556</v>
@@ -986,10 +1424,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C12" t="n">
         <v>0.0576</v>
@@ -1024,10 +1462,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C13" t="n">
         <v>0.6925</v>
@@ -1062,10 +1500,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C14" t="n">
         <v>0.3769</v>
@@ -1100,10 +1538,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C15" t="n">
         <v>-0.1158</v>
@@ -1138,10 +1576,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C16" t="n">
         <v>1</v>
@@ -1176,10 +1614,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C17" t="n">
         <v>-0.004</v>
@@ -1214,10 +1652,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C18" t="n">
         <v>0.6238</v>
@@ -1252,10 +1690,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C19" t="n">
         <v>-0.0312</v>
@@ -1290,10 +1728,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C20" t="n">
         <v>0.1696</v>
@@ -1328,10 +1766,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C21" t="n">
         <v>0.4556</v>
@@ -1366,10 +1804,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C22" t="n">
         <v>-0.004</v>
@@ -1404,10 +1842,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C23" t="n">
         <v>1</v>
@@ -1442,10 +1880,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C24" t="n">
         <v>-0.0135</v>
@@ -1480,10 +1918,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C25" t="n">
         <v>0.3289</v>
@@ -1518,10 +1956,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C26" t="n">
         <v>0.1973</v>
@@ -1556,10 +1994,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C27" t="n">
         <v>0.0576</v>
@@ -1594,10 +2032,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C28" t="n">
         <v>0.6238</v>
@@ -1632,10 +2070,10 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C29" t="n">
         <v>-0.0135</v>
@@ -1670,10 +2108,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C30" t="n">
         <v>1</v>
@@ -1708,10 +2146,10 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C31" t="n">
         <v>0.0239</v>
@@ -1746,10 +2184,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C32" t="n">
         <v>0.1087</v>
@@ -1784,10 +2222,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B33" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C33" t="n">
         <v>0.6925</v>
@@ -1822,10 +2260,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B34" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C34" t="n">
         <v>-0.0312</v>
@@ -1860,10 +2298,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B35" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C35" t="n">
         <v>0.3289</v>
@@ -1898,10 +2336,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C36" t="n">
         <v>0.0239</v>
@@ -1936,10 +2374,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B37" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C37" t="n">
         <v>1</v>

</xml_diff>